<commit_message>
Working on level 3 11:20pm
</commit_message>
<xml_diff>
--- a/Tabelas com os resultados dos testes -12-01-2025/Level3TestcaseReport.xlsx
+++ b/Tabelas com os resultados dos testes -12-01-2025/Level3TestcaseReport.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\class lectures\project\Tabelas com os resultados dos testes -12-01-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\class lectures\PRISEC III FINAL THESIS\Tabelas com os resultados dos testes -12-01-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="14400" windowHeight="7275" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="14400" windowHeight="7275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Level 3 Guest (1-100MB)" sheetId="13" r:id="rId1"/>
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,6 +190,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,11 +568,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="343194736"/>
-        <c:axId val="343195912"/>
+        <c:axId val="342815856"/>
+        <c:axId val="342820952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="343194736"/>
+        <c:axId val="342815856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343195912"/>
+        <c:crossAx val="342820952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343195912"/>
+        <c:axId val="342820952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343194736"/>
+        <c:crossAx val="342815856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -685,6 +688,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1108,11 +1112,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344194152"/>
-        <c:axId val="344191800"/>
+        <c:axId val="344208336"/>
+        <c:axId val="344202456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344194152"/>
+        <c:axId val="344208336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344191800"/>
+        <c:crossAx val="344202456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1163,7 +1167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344191800"/>
+        <c:axId val="344202456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344194152"/>
+        <c:crossAx val="344208336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1651,11 +1655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344191408"/>
-        <c:axId val="344192192"/>
+        <c:axId val="344203240"/>
+        <c:axId val="344205984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344191408"/>
+        <c:axId val="344203240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,7 +1702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344192192"/>
+        <c:crossAx val="344205984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1706,7 +1710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344192192"/>
+        <c:axId val="344205984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344191408"/>
+        <c:crossAx val="344203240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2194,11 +2198,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="343197088"/>
-        <c:axId val="343197872"/>
+        <c:axId val="344205592"/>
+        <c:axId val="344206768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="343197088"/>
+        <c:axId val="344205592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,7 +2245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343197872"/>
+        <c:crossAx val="344206768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2249,7 +2253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343197872"/>
+        <c:axId val="344206768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2300,7 +2304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343197088"/>
+        <c:crossAx val="344205592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2314,7 +2318,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3282,11 +3285,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="343196304"/>
-        <c:axId val="345607904"/>
+        <c:axId val="345586936"/>
+        <c:axId val="345586544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="343196304"/>
+        <c:axId val="345586936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3329,7 +3332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345607904"/>
+        <c:crossAx val="345586544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3337,7 +3340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345607904"/>
+        <c:axId val="345586544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3388,7 +3391,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343196304"/>
+        <c:crossAx val="345586936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3835,11 +3838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="343199832"/>
-        <c:axId val="343200616"/>
+        <c:axId val="342816248"/>
+        <c:axId val="342816640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="343199832"/>
+        <c:axId val="342816248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3882,7 +3885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343200616"/>
+        <c:crossAx val="342816640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3890,7 +3893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343200616"/>
+        <c:axId val="342816640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3941,7 +3944,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343199832"/>
+        <c:crossAx val="342816248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3955,6 +3958,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4306,11 +4310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="343198264"/>
-        <c:axId val="343195520"/>
+        <c:axId val="342818600"/>
+        <c:axId val="342819776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="343198264"/>
+        <c:axId val="342818600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4353,7 +4357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343195520"/>
+        <c:crossAx val="342819776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4361,7 +4365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343195520"/>
+        <c:axId val="342819776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4412,7 +4416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343198264"/>
+        <c:crossAx val="342818600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4426,6 +4430,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5023,11 +5028,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="343201792"/>
-        <c:axId val="343202184"/>
+        <c:axId val="342818992"/>
+        <c:axId val="342819384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="343201792"/>
+        <c:axId val="342818992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5070,7 +5075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343202184"/>
+        <c:crossAx val="342819384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5078,7 +5083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343202184"/>
+        <c:axId val="342819384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5129,7 +5134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343201792"/>
+        <c:crossAx val="342818992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5143,6 +5148,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5566,11 +5572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344194936"/>
-        <c:axId val="344196504"/>
+        <c:axId val="342820560"/>
+        <c:axId val="342821344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344194936"/>
+        <c:axId val="342820560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5613,7 +5619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344196504"/>
+        <c:crossAx val="342821344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5621,7 +5627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344196504"/>
+        <c:axId val="342821344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5672,7 +5678,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344194936"/>
+        <c:crossAx val="342820560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6109,11 +6115,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344190624"/>
-        <c:axId val="344192976"/>
+        <c:axId val="344209120"/>
+        <c:axId val="344203632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344190624"/>
+        <c:axId val="344209120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6156,7 +6162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344192976"/>
+        <c:crossAx val="344203632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6164,7 +6170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344192976"/>
+        <c:axId val="344203632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6215,7 +6221,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344190624"/>
+        <c:crossAx val="344209120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6652,11 +6658,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344194544"/>
-        <c:axId val="344196896"/>
+        <c:axId val="344209904"/>
+        <c:axId val="344207160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344194544"/>
+        <c:axId val="344209904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6699,7 +6705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344196896"/>
+        <c:crossAx val="344207160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6707,7 +6713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344196896"/>
+        <c:axId val="344207160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6758,7 +6764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344194544"/>
+        <c:crossAx val="344209904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7691,11 +7697,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="344197680"/>
-        <c:axId val="344198072"/>
+        <c:axId val="344205200"/>
+        <c:axId val="344204024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="344197680"/>
+        <c:axId val="344205200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7738,7 +7744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344198072"/>
+        <c:crossAx val="344204024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7746,7 +7752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344198072"/>
+        <c:axId val="344204024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7797,7 +7803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344197680"/>
+        <c:crossAx val="344205200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8259,11 +8265,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="344191016"/>
-        <c:axId val="344196112"/>
+        <c:axId val="344204808"/>
+        <c:axId val="344207552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344191016"/>
+        <c:axId val="344204808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8306,7 +8312,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344196112"/>
+        <c:crossAx val="344207552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8314,7 +8320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344196112"/>
+        <c:axId val="344207552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8365,7 +8371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344191016"/>
+        <c:crossAx val="344204808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16515,8 +16521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView topLeftCell="D15" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16528,11 +16534,28 @@
     <col min="6" max="6" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="2:3">
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="2:6" ht="14.25" customHeight="1">
+      <c r="B15" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -16882,7 +16905,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B15:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16893,8 +16916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="Q86" sqref="Q86"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="M95" sqref="M95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16906,11 +16929,21 @@
     <col min="6" max="6" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="2:3">
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="2:6" ht="14.25" customHeight="1">
+      <c r="B15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -17259,14 +17292,20 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="10"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
@@ -17616,8 +17655,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B15:F16"/>
+    <mergeCell ref="B42:F43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18716,7 +18755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView topLeftCell="A120" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
       <selection activeCell="Q144" sqref="Q144"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated files 01:14am 04/02/2025
</commit_message>
<xml_diff>
--- a/Tabelas com os resultados dos testes -12-01-2025/Level3TestcaseReport.xlsx
+++ b/Tabelas com os resultados dos testes -12-01-2025/Level3TestcaseReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="14400" windowHeight="7275" activeTab="1"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="14400" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="Level 3 Guest (1-100MB)" sheetId="13" r:id="rId1"/>
@@ -179,6 +179,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -190,9 +193,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,11 +568,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="342815856"/>
-        <c:axId val="342820952"/>
+        <c:axId val="334701600"/>
+        <c:axId val="334700032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="342815856"/>
+        <c:axId val="334701600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,7 +615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342820952"/>
+        <c:crossAx val="334700032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -623,7 +623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="342820952"/>
+        <c:axId val="334700032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342815856"/>
+        <c:crossAx val="334701600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1112,11 +1112,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344208336"/>
-        <c:axId val="344202456"/>
+        <c:axId val="335096512"/>
+        <c:axId val="335102392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344208336"/>
+        <c:axId val="335096512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,7 +1159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344202456"/>
+        <c:crossAx val="335102392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1167,7 +1167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344202456"/>
+        <c:axId val="335102392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344208336"/>
+        <c:crossAx val="335096512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1655,11 +1655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344203240"/>
-        <c:axId val="344205984"/>
+        <c:axId val="335097688"/>
+        <c:axId val="335097296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344203240"/>
+        <c:axId val="335097688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,7 +1702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344205984"/>
+        <c:crossAx val="335097296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1710,7 +1710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344205984"/>
+        <c:axId val="335097296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1761,7 +1761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344203240"/>
+        <c:crossAx val="335097688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2198,11 +2198,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344205592"/>
-        <c:axId val="344206768"/>
+        <c:axId val="335099648"/>
+        <c:axId val="335100040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344205592"/>
+        <c:axId val="335099648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2245,7 +2245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344206768"/>
+        <c:crossAx val="335100040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2253,7 +2253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344206768"/>
+        <c:axId val="335100040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2304,7 +2304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344205592"/>
+        <c:crossAx val="335099648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3285,11 +3285,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="345586936"/>
-        <c:axId val="345586544"/>
+        <c:axId val="352667848"/>
+        <c:axId val="352669808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345586936"/>
+        <c:axId val="352667848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3332,7 +3332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345586544"/>
+        <c:crossAx val="352669808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3340,7 +3340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345586544"/>
+        <c:axId val="352669808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3391,7 +3391,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345586936"/>
+        <c:crossAx val="352667848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3838,11 +3838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="342816248"/>
-        <c:axId val="342816640"/>
+        <c:axId val="334699248"/>
+        <c:axId val="334701992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="342816248"/>
+        <c:axId val="334699248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3885,7 +3885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342816640"/>
+        <c:crossAx val="334701992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3893,7 +3893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="342816640"/>
+        <c:axId val="334701992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3944,7 +3944,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342816248"/>
+        <c:crossAx val="334699248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4310,11 +4310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="342818600"/>
-        <c:axId val="342819776"/>
+        <c:axId val="334700424"/>
+        <c:axId val="334701208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="342818600"/>
+        <c:axId val="334700424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4357,7 +4357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342819776"/>
+        <c:crossAx val="334701208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4365,7 +4365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="342819776"/>
+        <c:axId val="334701208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4416,7 +4416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342818600"/>
+        <c:crossAx val="334700424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5028,11 +5028,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="342818992"/>
-        <c:axId val="342819384"/>
+        <c:axId val="334696504"/>
+        <c:axId val="334695328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="342818992"/>
+        <c:axId val="334696504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5075,7 +5075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342819384"/>
+        <c:crossAx val="334695328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5083,7 +5083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="342819384"/>
+        <c:axId val="334695328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5134,7 +5134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342818992"/>
+        <c:crossAx val="334696504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5572,11 +5572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="342820560"/>
-        <c:axId val="342821344"/>
+        <c:axId val="334697288"/>
+        <c:axId val="334697680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="342820560"/>
+        <c:axId val="334697288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5619,7 +5619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342821344"/>
+        <c:crossAx val="334697680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5627,7 +5627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="342821344"/>
+        <c:axId val="334697680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5678,7 +5678,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342820560"/>
+        <c:crossAx val="334697288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6115,11 +6115,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344209120"/>
-        <c:axId val="344203632"/>
+        <c:axId val="335099256"/>
+        <c:axId val="335100432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344209120"/>
+        <c:axId val="335099256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6162,7 +6162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344203632"/>
+        <c:crossAx val="335100432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6170,7 +6170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344203632"/>
+        <c:axId val="335100432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6221,7 +6221,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344209120"/>
+        <c:crossAx val="335099256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6658,11 +6658,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344209904"/>
-        <c:axId val="344207160"/>
+        <c:axId val="335094944"/>
+        <c:axId val="335096904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344209904"/>
+        <c:axId val="335094944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6705,7 +6705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344207160"/>
+        <c:crossAx val="335096904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6713,7 +6713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344207160"/>
+        <c:axId val="335096904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6764,7 +6764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344209904"/>
+        <c:crossAx val="335094944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7697,11 +7697,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="344205200"/>
-        <c:axId val="344204024"/>
+        <c:axId val="335095336"/>
+        <c:axId val="335101608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="344205200"/>
+        <c:axId val="335095336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7744,7 +7744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344204024"/>
+        <c:crossAx val="335101608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7752,7 +7752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344204024"/>
+        <c:axId val="335101608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7803,7 +7803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344205200"/>
+        <c:crossAx val="335095336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8265,11 +8265,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="344204808"/>
-        <c:axId val="344207552"/>
+        <c:axId val="335095728"/>
+        <c:axId val="335096120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344204808"/>
+        <c:axId val="335095728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8312,7 +8312,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344207552"/>
+        <c:crossAx val="335096120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8320,7 +8320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344207552"/>
+        <c:axId val="335096120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8371,7 +8371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344204808"/>
+        <c:crossAx val="335095728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16521,8 +16521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="D15" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16535,27 +16535,27 @@
   </cols>
   <sheetData>
     <row r="15" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -16916,8 +16916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="M95" sqref="M95"/>
+    <sheetView topLeftCell="A10" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16930,20 +16930,20 @@
   </cols>
   <sheetData>
     <row r="15" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -17292,20 +17292,20 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
@@ -17682,10 +17682,10 @@
   </cols>
   <sheetData>
     <row r="15" spans="2:3">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -18034,14 +18034,14 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="10"/>
+      <c r="C42" s="11"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
@@ -18769,10 +18769,10 @@
   </cols>
   <sheetData>
     <row r="15" spans="2:3">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -19121,14 +19121,14 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="10"/>
+      <c r="C42" s="11"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
@@ -19828,14 +19828,14 @@
       </c>
     </row>
     <row r="97" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B97" s="10" t="s">
+      <c r="B97" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C97" s="10"/>
+      <c r="C97" s="11"/>
     </row>
     <row r="98" spans="2:6">
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
     </row>
     <row r="100" spans="2:6">
       <c r="B100" s="3" t="s">

</xml_diff>